<commit_message>
add function google sheet
</commit_message>
<xml_diff>
--- a/ข้อมูล.xlsx
+++ b/ข้อมูล.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29122"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7556B70F-4DB7-43F1-85F1-56A78069D7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E37FB91-0F5B-46C9-A686-1F6D47866E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>แหนมเนืองกรุงเทพ</t>
   </si>
   <si>
-    <t>เลยแถวปากคลองตลาดใหม่ เลยปั๊ม pt ปั๊มปตท แล้วเลยร้านข้าผัดปูมาหน่อยเดียว</t>
+    <t>เลยปากคลองตลาดใหม่ เลยปั๊ม pt ปั๊มปตท แล้วเลยร้านข้าผัดปูมาหน่อยเดียว</t>
   </si>
   <si>
     <t>เปิด 10:00-18:00 เปิดทุกวัน</t>
@@ -60,88 +60,88 @@
     <t>เบอร์โทรร้าน 0979978256</t>
   </si>
   <si>
-    <t>มาซื้อหน้าร้านได้เลย จะจองไว้ก่อนก็ได้</t>
+    <t>มาซื้อหน้าร้านได้เลย จะจองไว้ก่อนก็ได้ แต่ถ้าจองชุดหั่นต้องจ่ายเงินก่อน</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ถ้าลูกค้าให้ส่ง เราจะเรียกไรเดอร์ส่งให้ </t>
+  </si>
+  <si>
+    <t>ค่าส่ง ลูกค้าส่งโลเคชั่นมาให้เราเช็คราคาค่าส่งให้ก่อน</t>
+  </si>
+  <si>
+    <t>ถ้าเราเช็คค่าส่งให้แล้วลูกค้าตกลง ขอชื่อและเบอร์โทรลูกค้าด้วย แล้วลูกค้าต้องโอนเงินก่อนเราถึงจะเรียกไรเดอร์มารับของไป</t>
+  </si>
+  <si>
+    <t>ถ้าจะโอนเงินส่ง QR ให้ลูกค้า</t>
+  </si>
+  <si>
+    <t>ถ้าลูกค้าขอสะสมแต้ม เดี๋ยวส่งให้ เพราะต้อง ส่งแบบแมนนวล</t>
+  </si>
+  <si>
+    <t>เมนู</t>
+  </si>
+  <si>
+    <t>บั๋นแส่ว</t>
+  </si>
+  <si>
+    <t>250 บาท</t>
+  </si>
+  <si>
+    <t>มีเฉพาะวันเสาร์-อาทิตย์</t>
+  </si>
+  <si>
+    <t>recommend</t>
+  </si>
+  <si>
+    <t>เมนูเวียดนามแท้ๆ ที่อร่อยไม่เหมือนใคร ต้องลอง! แป้งทอดห่อหมูผัดเน้นๆ รสเข้มข้น ทานคู่กับผักสดหลากชนิดแบบแน่นจาน แผ่นแป้งพิเศษ ไม่ต้องจุ่มน้ำ! ห่อสะดวก กินง่าย พร้อมจิ้มสูตรเด็ดครบรสในคำเดียว ทานง่าย ไม่ต้องเตรียมอะไรเพิ่ม แค่อร่อยอย่างเดียว!  ใครอยากเปิดโลกอาหารเวียดนามแท้ๆ ไม่จำเจ... ต้องลอง! </t>
+  </si>
+  <si>
+    <t>เมี่ยงปลาทูยักษ์</t>
+  </si>
+  <si>
+    <t>ปลาทูตัวใหญ่ยักษ์ โตเต็มคำ เสิร์ฟพร้อมผักสดจุกๆ ขนมจีนนุ่มๆ และน้ำจิ้มสูตรเด็ด แซ่บครบรสในคำเดียว</t>
+  </si>
+  <si>
+    <t>ไส้กรอกอีสานทอด</t>
+  </si>
+  <si>
+    <t>160 บาท</t>
+  </si>
+  <si>
+    <t>กุ้งพันอ้อย</t>
+  </si>
+  <si>
+    <t>340 บาท</t>
+  </si>
+  <si>
+    <t>กุ้งเน้นๆ พันแน่นบนอ้อย ย่างจนหอมกรุ่น เสิร์ฟคู่เส้นหมี่นุ่มๆ ราดกากหมูกรอบและหมูสามชั้นผัดสูตรพิเศษ เพิ่มความหอมด้วยกระเทียมเจียวกรุบกรอบ ทานคู่กับผักสดคัดพิเศษ พร้อมน้ำจิ้มเวียดนามรสเด็ด เปรี้ยวหวานเค็มกลมกล่อม เผ็ดพอดี  </t>
+  </si>
+  <si>
+    <t>แหนมเนืองชุดเล็ก 5 ไม้</t>
+  </si>
+  <si>
+    <t>320 บาท</t>
+  </si>
+  <si>
+    <t>ราคาแหนมเนืองเท่ากันทั้งแดงและวีที</t>
+  </si>
+  <si>
+    <t>ร้านเรามีจุดเด่นที่ให้ผักเยอะจุใจ และหลากหลายกว่า</t>
+  </si>
+  <si>
+    <t>แหนมเนืองชุดใหญ่ 10 ไม้</t>
+  </si>
+  <si>
+    <t>480 บาท</t>
+  </si>
+  <si>
+    <t>แหนมเนืองชุดพร้อมทาน 5 ไม้</t>
+  </si>
+  <si>
+    <t>แหนมเนืองพร้อมทาน เสิร์ฟพร้อมความสะดวกสบายในทุกคำ! ชุดนี้มาพร้อมหมูแหนมเนือง 5 ไม้ เนื้อแน่นเต็มคำ จัดเต็มผักสดหลากชนิดแบบจุใจ ที่ให้เยอะแบบจุกๆ! ทุกอย่าง หั่นและล้างสะอาดพร้อมทาน เสิร์ฟพร้อมแผ่นแป้งเหนียวนุ่ม  สด สะอาด หั่นสวย พร้อมกินทันที ไม่ต้องเตรียมเองให้ยุ่งยาก</t>
   </si>
   <si>
     <t>ถ้าสั่งชุดหั่นพร้อมทาน ลูกค้าต้องโอนเงินก่อน เราถึงจะทำให้ และเราใช้เวลาหั่นประมาณ 15 นาที ถ้ามารับช้าผลไม้อาจจะดำได้</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ถ้าลูกค้าให้ส่ง เราจะเรียกไรเดอร์ส่งให้ </t>
-  </si>
-  <si>
-    <t>ค่าส่ง ลูกค้าส่งโลเคชั่นมาให้เราเช็คราคาค่าส่งให้ก่อน</t>
-  </si>
-  <si>
-    <t>ถ้าเราเช็คค่าส่งให้แล้วลูกค้าตกลง ขอชื่อและเบอร์โทรลูกค้าด้วย แล้วลูกค้าต้องโอนเงินก่อนเราถึงจะเรียกไรเดอร์มารับของไป</t>
-  </si>
-  <si>
-    <t>ถ้าจะโอนเงินส่ง QR ให้ลูกค้า</t>
-  </si>
-  <si>
-    <t>ถ้าลูกค้าขอสะสมแต้ม เดี๋ยวส่งให้ เพราะต้อง ส่งแบบแมนนวล</t>
-  </si>
-  <si>
-    <t>เมนู</t>
-  </si>
-  <si>
-    <t>บั๋นแส่ว</t>
-  </si>
-  <si>
-    <t>250 บาท</t>
-  </si>
-  <si>
-    <t>มีเฉพาะวันเสาร์-อาทิตย์</t>
-  </si>
-  <si>
-    <t>recommend</t>
-  </si>
-  <si>
-    <t>เมนูเวียดนามแท้ๆ ที่อร่อยไม่เหมือนใคร ต้องลอง! แป้งทอดห่อหมูผัดเน้นๆ รสเข้มข้น ทานคู่กับผักสดหลากชนิดแบบแน่นจาน แผ่นแป้งพิเศษ ไม่ต้องจุ่มน้ำ! ห่อสะดวก กินง่าย พร้อมจิ้มสูตรเด็ดครบรสในคำเดียว ทานง่าย ไม่ต้องเตรียมอะไรเพิ่ม แค่อร่อยอย่างเดียว!  ใครอยากเปิดโลกอาหารเวียดนามแท้ๆ ไม่จำเจ... ต้องลอง! </t>
-  </si>
-  <si>
-    <t>เมี่ยงปลาทูยักษ์</t>
-  </si>
-  <si>
-    <t>ปลาทูตัวใหญ่ยักษ์ โตเต็มคำ เสิร์ฟพร้อมผักสดจุกๆ ขนมจีนนุ่มๆ และน้ำจิ้มสูตรเด็ด แซ่บครบรสในคำเดียว</t>
-  </si>
-  <si>
-    <t>ไส้กรอกอีสานทอด</t>
-  </si>
-  <si>
-    <t>160 บาท</t>
-  </si>
-  <si>
-    <t>กุ้งพันอ้อย</t>
-  </si>
-  <si>
-    <t>340 บาท</t>
-  </si>
-  <si>
-    <t>กุ้งเน้นๆ พันแน่นบนอ้อย ย่างจนหอมกรุ่น เสิร์ฟคู่เส้นหมี่นุ่มๆ ราดกากหมูกรอบและหมูสามชั้นผัดสูตรพิเศษ เพิ่มความหอมด้วยกระเทียมเจียวกรุบกรอบ ทานคู่กับผักสดคัดพิเศษ พร้อมน้ำจิ้มเวียดนามรสเด็ด เปรี้ยวหวานเค็มกลมกล่อม เผ็ดพอดี  </t>
-  </si>
-  <si>
-    <t>แหนมเนืองชุดเล็ก 5 ไม้</t>
-  </si>
-  <si>
-    <t>320 บาท</t>
-  </si>
-  <si>
-    <t>ราคาแหนมเนืองเท่ากันทั้งแดงและวีที</t>
-  </si>
-  <si>
-    <t>ร้านเรามีจุดเด่นที่ให้ผักเยอะจุใจ และหลากหลายกว่า</t>
-  </si>
-  <si>
-    <t>แหนมเนืองชุดใหญ่ 10 ไม้</t>
-  </si>
-  <si>
-    <t>480 บาท</t>
-  </si>
-  <si>
-    <t>แหนมเนืองชุดพร้อมทาน 5 ไม้</t>
-  </si>
-  <si>
-    <t>แหนมเนืองพร้อมทาน เสิร์ฟพร้อมความสะดวกสบายในทุกคำ! ชุดนี้มาพร้อมหมูแหนมเนือง 5 ไม้ เนื้อแน่นเต็มคำ จัดเต็มผักสดหลากชนิดแบบจุใจ ที่ให้เยอะแบบจุกๆ! ทุกอย่าง หั่นและล้างสะอาดพร้อมทาน เสิร์ฟพร้อมแผ่นแป้งเหนียวนุ่ม น้ำจิ้มรสเข้มข้นสูตรเฉพาะ  สด สะอาด หั่นสวย พร้อมกินทันที ไม่ต้องเตรียมเองให้ยุ่งยาก</t>
   </si>
   <si>
     <t>หมูยอ</t>
@@ -182,7 +182,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="187" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -234,7 +234,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -242,7 +242,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -255,55 +255,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1752600</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>2676525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49A05F94-66D7-4DD9-B06D-FA5FD81A6217}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3400425" y="7058025"/>
-          <a:ext cx="1676400" cy="2638425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -638,14 +589,15 @@
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="81.75" customHeight="1">
+    <row r="2" spans="1:8" ht="81.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -659,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="66.75" customHeight="1">
+    <row r="3" spans="1:8" ht="66.75" customHeight="1">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -670,227 +622,226 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="80.25" customHeight="1">
+    <row r="5" spans="1:8" ht="31.5">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="82.5" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="82.5" customHeight="1">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75">
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="216" customHeight="1">
+    <row r="8" spans="1:8" ht="32.25">
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="32.25">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="129">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="129">
-      <c r="A11" t="s">
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="15.75">
+      <c r="A12"/>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="96">
       <c r="A13"/>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="E13"/>
-      <c r="F13"/>
+      <c r="F13" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="96">
-      <c r="A14"/>
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="47.25">
       <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="47.25">
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="111.75">
+      <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="47.25">
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="F16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="47.25">
-      <c r="B16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="129">
-      <c r="B17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="H16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>32</v>
-      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17"/>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1">
       <c r="B18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" s="1"/>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D19"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A21" s="1"/>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="B22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
         <v>47</v>
       </c>
     </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>